<commit_message>
Exercicio mod-19: (08/08/2024) Exercicio mod-20: (08/08/2024) Desenvolvendo: - Tela Detalhes - Carosel - Botão voltar
</commit_message>
<xml_diff>
--- a/Chamados Tutor.xlsx
+++ b/Chamados Tutor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\CursoAndroidStudioKotlin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14ED5EC9-79F6-48F9-8562-48C268313381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07725E6-C32F-488F-9DB7-06446462DA72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D03A6DA7-1C8A-419E-A94D-75669D229CD0}"/>
+    <workbookView xWindow="14805" yWindow="1965" windowWidth="14055" windowHeight="12585" xr2:uid="{D03A6DA7-1C8A-419E-A94D-75669D229CD0}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>CURSO EBAC</t>
   </si>
@@ -66,6 +66,27 @@
   </si>
   <si>
     <t>hqawasomeapp</t>
+  </si>
+  <si>
+    <t>20.3</t>
+  </si>
+  <si>
+    <t>Aula 3: Hands On - Parte 1</t>
+  </si>
+  <si>
+    <t>Ticket</t>
+  </si>
+  <si>
+    <t>#BR-66230</t>
+  </si>
+  <si>
+    <t>Exercicio</t>
+  </si>
+  <si>
+    <t>#BR-65851</t>
+  </si>
+  <si>
+    <t>TMDB</t>
   </si>
 </sst>
 </file>
@@ -494,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E93A04C7-9F76-426A-8E37-1343291D63A6}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,21 +527,22 @@
     <col min="3" max="3" width="8.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="28" style="4" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="6" max="6" width="20" style="4" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
@@ -539,8 +561,11 @@
       <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
+      <c r="G4" s="8" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>45503</v>
       </c>
@@ -561,17 +586,50 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>45509</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="D6" s="3">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>45511</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="18" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,7 +650,9 @@
     <row r="34" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="36" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>